<commit_message>
adding data sheet and excel read functionality for the dataprovider
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\eclipse-workspace\dockerValidation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D71309-0DF5-4F3A-9419-BA1222594E01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +26,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+  <si>
+    <t>Greeting</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>bye</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>solo</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>hi sheet 3</t>
+  </si>
+  <si>
+    <t>bye sheet 3</t>
+  </si>
+  <si>
+    <t>sheet 3 text to prove the first row</t>
+  </si>
+  <si>
+    <t>sheet 3 text to prove the second row</t>
+  </si>
+  <si>
+    <t>howdy sheet 2</t>
+  </si>
+  <si>
+    <t>later sheet 2</t>
+  </si>
+  <si>
+    <t>what up sheet 2</t>
+  </si>
+  <si>
+    <t>sup sheet 2</t>
+  </si>
+  <si>
+    <t>sheet 2 row 1</t>
+  </si>
+  <si>
+    <t>sheet 2 row 2</t>
+  </si>
+  <si>
+    <t>sheet 2 row 3</t>
+  </si>
+  <si>
+    <t>sheet 2 row 4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,13 +412,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="13.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>7689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B303C2-7D05-45A3-A1E1-CC126263E491}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3845C4D-015F-4FB4-90CD-5F6990466AEE}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="13.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>75867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>970600</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>